<commit_message>
SIRS models for each population
</commit_message>
<xml_diff>
--- a/SIRS MODELS/spain.xlsx
+++ b/SIRS MODELS/spain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlour\Desktop\COVID19\SIRS MODELS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283B3938-2B1B-41A5-B2EE-A3C8789BDDAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436E53E-0E67-4A67-BBD4-0AB38DFFB13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6825,8 +6825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:W426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="B2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>